<commit_message>
Updates to clean-index.pl and process-images.ol
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fraser Bennett\Documents\SIL LEAD\CAI ACR AF\illustrations\update files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fraser Bennett\source\repos\ACR-Illustrations-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBD9544-2F03-4A29-BCFB-C3113F247679}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C33AEE4-BCBF-427E-B98E-4EF4C855BC35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="0" windowWidth="14145" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4560" yWindow="0" windowWidth="14145" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="4" r:id="rId1"/>
@@ -303,7 +303,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>